<commit_message>
added Excel write file but has error
</commit_message>
<xml_diff>
--- a/TestData/PolicyBazar_UserData.xlsx
+++ b/TestData/PolicyBazar_UserData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anura\eclipse-workspace\Hack\Hackathon_Project\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C803B239-DF34-4CF3-91CC-DAB34F4F6C3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C53B2652-47DA-44E5-82A0-64A1DD0863F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2640" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,27 +21,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>Name</t>
+    <t>Company</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Phone Number</t>
-  </si>
-  <si>
-    <t>Anurag</t>
-  </si>
-  <si>
-    <t>anu123@gmail.com</t>
-  </si>
-  <si>
-    <t>Travel Country</t>
-  </si>
-  <si>
-    <t>United Kingdom</t>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
@@ -69,7 +50,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +60,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -96,13 +83,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -387,7 +375,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,31 +393,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>9638527415</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{51D6C41E-7713-455B-B440-4A2DAECBD0CB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>